<commit_message>
Updating hitters, pitcher_season_stats and pitchers
</commit_message>
<xml_diff>
--- a/api/pitcher_season_stats.xlsx
+++ b/api/pitcher_season_stats.xlsx
@@ -1687,31 +1687,31 @@
         <v>23</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>4</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J4">
         <v>65.2</v>
       </c>
       <c r="K4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L4">
+        <v>42</v>
+      </c>
+      <c r="M4">
+        <v>35</v>
+      </c>
+      <c r="N4">
         <v>37</v>
-      </c>
-      <c r="M4">
-        <v>30</v>
-      </c>
-      <c r="N4">
-        <v>33</v>
       </c>
       <c r="O4">
         <v>68</v>
@@ -1720,16 +1720,16 @@
         <v>10</v>
       </c>
       <c r="Q4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R4">
-        <v>4.11</v>
+        <v>4.8</v>
       </c>
       <c r="S4">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="T4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="U4">
         <v>2</v>
@@ -1753,13 +1753,13 @@
         <v>1</v>
       </c>
       <c r="AB4">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="AC4">
-        <v>1169</v>
+        <v>1194</v>
       </c>
       <c r="AD4">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE4">
         <v>15</v>
@@ -1777,16 +1777,16 @@
         <v>11</v>
       </c>
       <c r="AJ4">
-        <v>1.416</v>
+        <v>1.492</v>
       </c>
       <c r="AK4">
-        <v>0.284</v>
+        <v>0.288</v>
       </c>
       <c r="AL4">
         <v>9.300000000000001</v>
       </c>
       <c r="AM4">
-        <v>2.06</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="5" spans="1:39">
@@ -2371,7 +2371,7 @@
         <v>31</v>
       </c>
       <c r="E10">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -2383,22 +2383,22 @@
         <v>3</v>
       </c>
       <c r="J10">
-        <v>47.1</v>
+        <v>49</v>
       </c>
       <c r="K10">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L10">
+        <v>28</v>
+      </c>
+      <c r="M10">
         <v>25</v>
       </c>
-      <c r="M10">
-        <v>22</v>
-      </c>
       <c r="N10">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O10">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P10">
         <v>5</v>
@@ -2407,13 +2407,13 @@
         <v>3</v>
       </c>
       <c r="R10">
-        <v>4.18</v>
+        <v>4.59</v>
       </c>
       <c r="S10">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="T10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U10">
         <v>5</v>
@@ -2422,7 +2422,7 @@
         <v>1</v>
       </c>
       <c r="W10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X10">
         <v>1</v>
@@ -2437,10 +2437,10 @@
         <v>0</v>
       </c>
       <c r="AB10">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="AC10">
-        <v>731</v>
+        <v>784</v>
       </c>
       <c r="AD10">
         <v>68</v>
@@ -2455,22 +2455,22 @@
         <v>51</v>
       </c>
       <c r="AH10">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AI10">
         <v>6</v>
       </c>
       <c r="AJ10">
-        <v>1.204</v>
+        <v>1.286</v>
       </c>
       <c r="AK10">
-        <v>0.277</v>
+        <v>0.294</v>
       </c>
       <c r="AL10">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="AM10">
-        <v>2.71</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="11" spans="1:39">
@@ -2487,49 +2487,49 @@
         <v>25</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F11">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <v>4</v>
       </c>
       <c r="J11">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="K11">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="L11">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="M11">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="N11">
         <v>22</v>
       </c>
       <c r="O11">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="P11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11">
-        <v>2.31</v>
+        <v>2.61</v>
       </c>
       <c r="S11">
-        <v>253</v>
+        <v>278</v>
       </c>
       <c r="T11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U11">
         <v>2</v>
@@ -2553,16 +2553,16 @@
         <v>0</v>
       </c>
       <c r="AB11">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="AC11">
-        <v>1055</v>
+        <v>1157</v>
       </c>
       <c r="AD11">
         <v>63</v>
       </c>
       <c r="AE11">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AF11">
         <v>11</v>
@@ -2577,16 +2577,16 @@
         <v>8</v>
       </c>
       <c r="AJ11">
-        <v>1</v>
+        <v>1.013</v>
       </c>
       <c r="AK11">
-        <v>0.218</v>
+        <v>0.225</v>
       </c>
       <c r="AL11">
-        <v>7.5</v>
+        <v>7.7</v>
       </c>
       <c r="AM11">
-        <v>2.64</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="12" spans="1:39">
@@ -2716,49 +2716,49 @@
         <v>25</v>
       </c>
       <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
         <v>10</v>
       </c>
-      <c r="F13">
-        <v>9</v>
-      </c>
       <c r="G13">
         <v>3</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J13">
-        <v>48</v>
+        <v>53.1</v>
       </c>
       <c r="K13">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L13">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="M13">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N13">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O13">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P13">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q13">
         <v>4</v>
       </c>
       <c r="R13">
-        <v>5.25</v>
+        <v>5.4</v>
       </c>
       <c r="S13">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="T13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -2782,13 +2782,13 @@
         <v>2</v>
       </c>
       <c r="AB13">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="AC13">
-        <v>801</v>
+        <v>882</v>
       </c>
       <c r="AD13">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AE13">
         <v>13</v>
@@ -2797,7 +2797,7 @@
         <v>13</v>
       </c>
       <c r="AG13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AH13">
         <v>20</v>
@@ -2806,16 +2806,16 @@
         <v>10</v>
       </c>
       <c r="AJ13">
-        <v>1.313</v>
+        <v>1.275</v>
       </c>
       <c r="AK13">
-        <v>0.292</v>
+        <v>0.275</v>
       </c>
       <c r="AL13">
-        <v>9</v>
+        <v>8.9</v>
       </c>
       <c r="AM13">
-        <v>2.67</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="14" spans="1:39">
@@ -3409,34 +3409,34 @@
         <v>24</v>
       </c>
       <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
         <v>4</v>
       </c>
-      <c r="F19">
-        <v>3</v>
-      </c>
       <c r="G19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="J19">
-        <v>21.1</v>
+        <v>28.1</v>
       </c>
       <c r="K19">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="L19">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M19">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N19">
         <v>3</v>
       </c>
       <c r="O19">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P19">
         <v>2</v>
@@ -3445,10 +3445,10 @@
         <v>1</v>
       </c>
       <c r="R19">
-        <v>4.22</v>
+        <v>3.81</v>
       </c>
       <c r="S19">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="T19">
         <v>2</v>
@@ -3460,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X19">
         <v>0</v>
@@ -3469,46 +3469,46 @@
         <v>0</v>
       </c>
       <c r="Z19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA19">
         <v>0</v>
       </c>
       <c r="AB19">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="AC19">
-        <v>334</v>
+        <v>425</v>
       </c>
       <c r="AD19">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AE19">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AF19">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AG19">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="AH19">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AJ19">
-        <v>1.031</v>
+        <v>1.024</v>
       </c>
       <c r="AK19">
-        <v>0.266</v>
+        <v>0.273</v>
       </c>
       <c r="AL19">
-        <v>6.8</v>
+        <v>5.4</v>
       </c>
       <c r="AM19">
-        <v>5.33</v>
+        <v>5.67</v>
       </c>
     </row>
     <row r="20" spans="1:39">
@@ -4090,22 +4090,22 @@
         <v>23</v>
       </c>
       <c r="E25">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F25">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H25">
         <v>8</v>
       </c>
       <c r="J25">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="K25">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L25">
         <v>30</v>
@@ -4114,25 +4114,25 @@
         <v>27</v>
       </c>
       <c r="N25">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O25">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="P25">
         <v>6</v>
       </c>
       <c r="Q25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R25">
-        <v>2.01</v>
+        <v>1.91</v>
       </c>
       <c r="S25">
-        <v>435</v>
+        <v>456</v>
       </c>
       <c r="T25">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="U25">
         <v>1</v>
@@ -4156,10 +4156,10 @@
         <v>2</v>
       </c>
       <c r="AB25">
-        <v>469</v>
+        <v>492</v>
       </c>
       <c r="AC25">
-        <v>1901</v>
+        <v>1987</v>
       </c>
       <c r="AD25">
         <v>65</v>
@@ -4177,19 +4177,19 @@
         <v>23</v>
       </c>
       <c r="AI25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AJ25">
-        <v>0.926</v>
+        <v>0.913</v>
       </c>
       <c r="AK25">
-        <v>0.255</v>
+        <v>0.252</v>
       </c>
       <c r="AL25">
         <v>9.699999999999999</v>
       </c>
       <c r="AM25">
-        <v>4.37</v>
+        <v>4.42</v>
       </c>
     </row>
     <row r="26" spans="1:39">
@@ -4893,34 +4893,34 @@
         <v>26</v>
       </c>
       <c r="E32">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F32">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H32">
         <v>6</v>
       </c>
       <c r="J32">
-        <v>79.2</v>
+        <v>84.2</v>
       </c>
       <c r="K32">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="L32">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="M32">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N32">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O32">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P32">
         <v>16</v>
@@ -4929,13 +4929,13 @@
         <v>4</v>
       </c>
       <c r="R32">
-        <v>5.65</v>
+        <v>5.63</v>
       </c>
       <c r="S32">
-        <v>321</v>
+        <v>342</v>
       </c>
       <c r="T32">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="U32">
         <v>1</v>
@@ -4944,10 +4944,10 @@
         <v>0</v>
       </c>
       <c r="W32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y32">
         <v>9</v>
@@ -4959,22 +4959,22 @@
         <v>0</v>
       </c>
       <c r="AB32">
-        <v>356</v>
+        <v>381</v>
       </c>
       <c r="AC32">
-        <v>1326</v>
+        <v>1434</v>
       </c>
       <c r="AD32">
         <v>62</v>
       </c>
       <c r="AE32">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AF32">
         <v>9</v>
       </c>
       <c r="AG32">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AH32">
         <v>25</v>
@@ -4983,16 +4983,16 @@
         <v>1</v>
       </c>
       <c r="AJ32">
-        <v>1.506</v>
+        <v>1.547</v>
       </c>
       <c r="AK32">
-        <v>0.319</v>
+        <v>0.324</v>
       </c>
       <c r="AL32">
-        <v>7.8</v>
+        <v>7.4</v>
       </c>
       <c r="AM32">
-        <v>2.46</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="33" spans="1:39">
@@ -8438,49 +8438,49 @@
         <v>25</v>
       </c>
       <c r="E63">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F63">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G63">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H63">
         <v>6</v>
       </c>
       <c r="J63">
-        <v>80.09999999999999</v>
+        <v>86.09999999999999</v>
       </c>
       <c r="K63">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="L63">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M63">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="N63">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="O63">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="P63">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R63">
-        <v>4.37</v>
+        <v>4.27</v>
       </c>
       <c r="S63">
-        <v>305</v>
+        <v>327</v>
       </c>
       <c r="T63">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="U63">
         <v>0</v>
@@ -8504,40 +8504,40 @@
         <v>0</v>
       </c>
       <c r="AB63">
-        <v>346</v>
+        <v>373</v>
       </c>
       <c r="AC63">
-        <v>1383</v>
+        <v>1478</v>
       </c>
       <c r="AD63">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AE63">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AF63">
         <v>10</v>
       </c>
       <c r="AG63">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH63">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AI63">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AJ63">
-        <v>1.357</v>
+        <v>1.355</v>
       </c>
       <c r="AK63">
-        <v>0.269</v>
+        <v>0.266</v>
       </c>
       <c r="AL63">
-        <v>7.7</v>
+        <v>7.9</v>
       </c>
       <c r="AM63">
-        <v>1.82</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="64" spans="1:39">
@@ -9479,10 +9479,10 @@
         <v>26</v>
       </c>
       <c r="E72">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F72">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G72">
         <v>3</v>
@@ -9491,34 +9491,34 @@
         <v>4</v>
       </c>
       <c r="J72">
-        <v>94.2</v>
+        <v>99</v>
       </c>
       <c r="K72">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="L72">
+        <v>42</v>
+      </c>
+      <c r="M72">
         <v>41</v>
       </c>
-      <c r="M72">
-        <v>40</v>
-      </c>
       <c r="N72">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O72">
         <v>50</v>
       </c>
       <c r="P72">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q72">
         <v>6</v>
       </c>
       <c r="R72">
-        <v>3.8</v>
+        <v>3.73</v>
       </c>
       <c r="S72">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="T72">
         <v>13</v>
@@ -9530,7 +9530,7 @@
         <v>1</v>
       </c>
       <c r="W72">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X72">
         <v>4</v>
@@ -9545,10 +9545,10 @@
         <v>2</v>
       </c>
       <c r="AB72">
-        <v>412</v>
+        <v>431</v>
       </c>
       <c r="AC72">
-        <v>1552</v>
+        <v>1620</v>
       </c>
       <c r="AD72">
         <v>62</v>
@@ -9569,16 +9569,16 @@
         <v>13</v>
       </c>
       <c r="AJ72">
-        <v>1.394</v>
+        <v>1.414</v>
       </c>
       <c r="AK72">
-        <v>0.248</v>
+        <v>0.254</v>
       </c>
       <c r="AL72">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="AM72">
-        <v>1.09</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="73" spans="1:39">
@@ -9943,10 +9943,10 @@
         <v>25</v>
       </c>
       <c r="E76">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F76">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G76">
         <v>4</v>
@@ -9955,22 +9955,22 @@
         <v>8</v>
       </c>
       <c r="J76">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="K76">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="L76">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M76">
         <v>47</v>
       </c>
       <c r="N76">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="O76">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="P76">
         <v>16</v>
@@ -9979,13 +9979,13 @@
         <v>5</v>
       </c>
       <c r="R76">
-        <v>4.36</v>
+        <v>4.19</v>
       </c>
       <c r="S76">
-        <v>371</v>
+        <v>387</v>
       </c>
       <c r="T76">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U76">
         <v>1</v>
@@ -10000,7 +10000,7 @@
         <v>3</v>
       </c>
       <c r="Y76">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Z76">
         <v>5</v>
@@ -10009,13 +10009,13 @@
         <v>4</v>
       </c>
       <c r="AB76">
-        <v>424</v>
+        <v>444</v>
       </c>
       <c r="AC76">
-        <v>1639</v>
+        <v>1728</v>
       </c>
       <c r="AD76">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AE76">
         <v>15</v>
@@ -10024,25 +10024,25 @@
         <v>10</v>
       </c>
       <c r="AG76">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AH76">
         <v>24</v>
       </c>
       <c r="AI76">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AJ76">
-        <v>1.402</v>
+        <v>1.416</v>
       </c>
       <c r="AK76">
         <v>0.277</v>
       </c>
       <c r="AL76">
-        <v>7.4</v>
+        <v>7.6</v>
       </c>
       <c r="AM76">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="77" spans="1:39">
@@ -10175,7 +10175,7 @@
         <v>25</v>
       </c>
       <c r="E78">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -10184,23 +10184,23 @@
         <v>3</v>
       </c>
       <c r="J78">
-        <v>31.1</v>
+        <v>32.1</v>
       </c>
       <c r="K78">
+        <v>29</v>
+      </c>
+      <c r="L78">
+        <v>20</v>
+      </c>
+      <c r="M78">
+        <v>14</v>
+      </c>
+      <c r="N78">
+        <v>17</v>
+      </c>
+      <c r="O78">
         <v>26</v>
       </c>
-      <c r="L78">
-        <v>19</v>
-      </c>
-      <c r="M78">
-        <v>13</v>
-      </c>
-      <c r="N78">
-        <v>15</v>
-      </c>
-      <c r="O78">
-        <v>24</v>
-      </c>
       <c r="P78">
         <v>2</v>
       </c>
@@ -10208,13 +10208,13 @@
         <v>2</v>
       </c>
       <c r="R78">
-        <v>3.73</v>
+        <v>3.9</v>
       </c>
       <c r="S78">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="T78">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="U78">
         <v>0</v>
@@ -10226,7 +10226,7 @@
         <v>3</v>
       </c>
       <c r="X78">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y78">
         <v>1</v>
@@ -10238,10 +10238,10 @@
         <v>0</v>
       </c>
       <c r="AB78">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="AC78">
-        <v>535</v>
+        <v>565</v>
       </c>
       <c r="AD78">
         <v>60</v>
@@ -10253,25 +10253,25 @@
         <v>7</v>
       </c>
       <c r="AG78">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AH78">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="AI78">
         <v>2</v>
       </c>
       <c r="AJ78">
-        <v>1.309</v>
+        <v>1.423</v>
       </c>
       <c r="AK78">
-        <v>0.255</v>
+        <v>0.276</v>
       </c>
       <c r="AL78">
-        <v>6.9</v>
+        <v>7.2</v>
       </c>
       <c r="AM78">
-        <v>1.6</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="79" spans="1:39">
@@ -10987,7 +10987,7 @@
         <v>25</v>
       </c>
       <c r="E85">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -10996,7 +10996,7 @@
         <v>2</v>
       </c>
       <c r="J85">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K85">
         <v>24</v>
@@ -11008,10 +11008,10 @@
         <v>7</v>
       </c>
       <c r="N85">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O85">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P85">
         <v>1</v>
@@ -11020,10 +11020,10 @@
         <v>0</v>
       </c>
       <c r="R85">
-        <v>2.74</v>
+        <v>2.63</v>
       </c>
       <c r="S85">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="T85">
         <v>8</v>
@@ -11050,10 +11050,10 @@
         <v>0</v>
       </c>
       <c r="AB85">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="AC85">
-        <v>388</v>
+        <v>401</v>
       </c>
       <c r="AD85">
         <v>66</v>
@@ -11062,10 +11062,10 @@
         <v>16</v>
       </c>
       <c r="AF85">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AG85">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AH85">
         <v>21</v>
@@ -11074,16 +11074,16 @@
         <v>1</v>
       </c>
       <c r="AJ85">
-        <v>1.478</v>
+        <v>1.458</v>
       </c>
       <c r="AK85">
-        <v>0.329</v>
+        <v>0.319</v>
       </c>
       <c r="AL85">
-        <v>7.4</v>
+        <v>7.5</v>
       </c>
       <c r="AM85">
-        <v>1.9</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="86" spans="1:39">
@@ -11448,7 +11448,7 @@
         <v>25</v>
       </c>
       <c r="E89">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F89">
         <v>14</v>
@@ -11457,40 +11457,40 @@
         <v>4</v>
       </c>
       <c r="H89">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J89">
-        <v>79.09999999999999</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="K89">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="L89">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="M89">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="N89">
         <v>27</v>
       </c>
       <c r="O89">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="P89">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Q89">
         <v>4</v>
       </c>
       <c r="R89">
-        <v>6.13</v>
+        <v>6.48</v>
       </c>
       <c r="S89">
-        <v>327</v>
+        <v>346</v>
       </c>
       <c r="T89">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U89">
         <v>4</v>
@@ -11505,7 +11505,7 @@
         <v>1</v>
       </c>
       <c r="Y89">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z89">
         <v>0</v>
@@ -11514,10 +11514,10 @@
         <v>0</v>
       </c>
       <c r="AB89">
-        <v>359</v>
+        <v>378</v>
       </c>
       <c r="AC89">
-        <v>1336</v>
+        <v>1399</v>
       </c>
       <c r="AD89">
         <v>66</v>
@@ -11526,7 +11526,7 @@
         <v>18</v>
       </c>
       <c r="AF89">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AG89">
         <v>42</v>
@@ -11538,16 +11538,16 @@
         <v>6</v>
       </c>
       <c r="AJ89">
-        <v>1.525</v>
+        <v>1.536</v>
       </c>
       <c r="AK89">
-        <v>0.362</v>
+        <v>0.363</v>
       </c>
       <c r="AL89">
         <v>10.3</v>
       </c>
       <c r="AM89">
-        <v>3.37</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="90" spans="1:39">
@@ -11793,7 +11793,7 @@
         <v>29</v>
       </c>
       <c r="E92">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F92">
         <v>0</v>
@@ -11808,7 +11808,7 @@
         <v>1</v>
       </c>
       <c r="J92">
-        <v>46.1</v>
+        <v>47.1</v>
       </c>
       <c r="K92">
         <v>35</v>
@@ -11823,7 +11823,7 @@
         <v>19</v>
       </c>
       <c r="O92">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="P92">
         <v>2</v>
@@ -11832,10 +11832,10 @@
         <v>4</v>
       </c>
       <c r="R92">
-        <v>3.3</v>
+        <v>3.23</v>
       </c>
       <c r="S92">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="T92">
         <v>6</v>
@@ -11862,10 +11862,10 @@
         <v>0</v>
       </c>
       <c r="AB92">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="AC92">
-        <v>815</v>
+        <v>828</v>
       </c>
       <c r="AD92">
         <v>65</v>
@@ -11874,7 +11874,7 @@
         <v>16</v>
       </c>
       <c r="AF92">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AG92">
         <v>47</v>
@@ -11886,16 +11886,16 @@
         <v>3</v>
       </c>
       <c r="AJ92">
-        <v>1.165</v>
+        <v>1.141</v>
       </c>
       <c r="AK92">
         <v>0.3</v>
       </c>
       <c r="AL92">
-        <v>11.3</v>
+        <v>11.6</v>
       </c>
       <c r="AM92">
-        <v>3.05</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="93" spans="1:39">
@@ -11912,49 +11912,49 @@
         <v>26</v>
       </c>
       <c r="E93">
+        <v>12</v>
+      </c>
+      <c r="F93">
         <v>11</v>
       </c>
-      <c r="F93">
-        <v>10</v>
-      </c>
       <c r="G93">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H93">
         <v>2</v>
       </c>
       <c r="J93">
-        <v>52</v>
+        <v>57.2</v>
       </c>
       <c r="K93">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L93">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M93">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N93">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="O93">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P93">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q93">
         <v>1</v>
       </c>
       <c r="R93">
-        <v>4.67</v>
+        <v>4.53</v>
       </c>
       <c r="S93">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="T93">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="U93">
         <v>1</v>
@@ -11966,10 +11966,10 @@
         <v>2</v>
       </c>
       <c r="X93">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y93">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z93">
         <v>0</v>
@@ -11978,10 +11978,10 @@
         <v>0</v>
       </c>
       <c r="AB93">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="AC93">
-        <v>861</v>
+        <v>950</v>
       </c>
       <c r="AD93">
         <v>68</v>
@@ -11993,7 +11993,7 @@
         <v>8</v>
       </c>
       <c r="AG93">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH93">
         <v>30</v>
@@ -12002,16 +12002,16 @@
         <v>10</v>
       </c>
       <c r="AJ93">
-        <v>1.423</v>
+        <v>1.439</v>
       </c>
       <c r="AK93">
-        <v>0.34</v>
+        <v>0.337</v>
       </c>
       <c r="AL93">
-        <v>7.6</v>
+        <v>7.5</v>
       </c>
       <c r="AM93">
-        <v>4.89</v>
+        <v>4.36</v>
       </c>
     </row>
     <row r="94" spans="1:39">
@@ -12028,46 +12028,46 @@
         <v>26</v>
       </c>
       <c r="E94">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F94">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G94">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H94">
         <v>9</v>
       </c>
       <c r="J94">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="K94">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="L94">
+        <v>60</v>
+      </c>
+      <c r="M94">
         <v>55</v>
-      </c>
-      <c r="M94">
-        <v>52</v>
       </c>
       <c r="N94">
         <v>33</v>
       </c>
       <c r="O94">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="P94">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q94">
         <v>7</v>
       </c>
       <c r="R94">
-        <v>4.29</v>
+        <v>4.27</v>
       </c>
       <c r="S94">
-        <v>412</v>
+        <v>439</v>
       </c>
       <c r="T94">
         <v>13</v>
@@ -12079,13 +12079,13 @@
         <v>1</v>
       </c>
       <c r="W94">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X94">
         <v>2</v>
       </c>
       <c r="Y94">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Z94">
         <v>3</v>
@@ -12094,13 +12094,13 @@
         <v>3</v>
       </c>
       <c r="AB94">
-        <v>456</v>
+        <v>483</v>
       </c>
       <c r="AC94">
-        <v>1818</v>
+        <v>1904</v>
       </c>
       <c r="AD94">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AE94">
         <v>18</v>
@@ -12112,22 +12112,22 @@
         <v>45</v>
       </c>
       <c r="AH94">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AI94">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AJ94">
-        <v>1.239</v>
+        <v>1.216</v>
       </c>
       <c r="AK94">
-        <v>0.281</v>
+        <v>0.278</v>
       </c>
       <c r="AL94">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
       <c r="AM94">
-        <v>2.88</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:39">
@@ -13054,10 +13054,10 @@
         <v>32</v>
       </c>
       <c r="E103">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F103">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G103">
         <v>7</v>
@@ -13066,37 +13066,37 @@
         <v>3</v>
       </c>
       <c r="J103">
-        <v>77.2</v>
+        <v>80.2</v>
       </c>
       <c r="K103">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L103">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="M103">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N103">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O103">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="P103">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q103">
         <v>1</v>
       </c>
       <c r="R103">
-        <v>1.39</v>
+        <v>1.79</v>
       </c>
       <c r="S103">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="T103">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U103">
         <v>4</v>
@@ -13120,13 +13120,13 @@
         <v>0</v>
       </c>
       <c r="AB103">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="AC103">
-        <v>1243</v>
+        <v>1316</v>
       </c>
       <c r="AD103">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE103">
         <v>15</v>
@@ -13144,16 +13144,16 @@
         <v>6</v>
       </c>
       <c r="AJ103">
-        <v>1.133</v>
+        <v>1.178</v>
       </c>
       <c r="AK103">
-        <v>0.256</v>
+        <v>0.262</v>
       </c>
       <c r="AL103">
-        <v>8.6</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="AM103">
-        <v>2.24</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="104" spans="1:39">
@@ -13286,7 +13286,7 @@
         <v>25</v>
       </c>
       <c r="E105">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -13301,34 +13301,34 @@
         <v>2</v>
       </c>
       <c r="J105">
-        <v>44.1</v>
+        <v>45.1</v>
       </c>
       <c r="K105">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L105">
+        <v>22</v>
+      </c>
+      <c r="M105">
         <v>21</v>
-      </c>
-      <c r="M105">
-        <v>20</v>
       </c>
       <c r="N105">
         <v>19</v>
       </c>
       <c r="O105">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P105">
         <v>4</v>
       </c>
       <c r="Q105">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R105">
-        <v>4.06</v>
+        <v>4.17</v>
       </c>
       <c r="S105">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="T105">
         <v>8</v>
@@ -13346,7 +13346,7 @@
         <v>0</v>
       </c>
       <c r="Y105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z105">
         <v>2</v>
@@ -13355,10 +13355,10 @@
         <v>0</v>
       </c>
       <c r="AB105">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="AC105">
-        <v>773</v>
+        <v>792</v>
       </c>
       <c r="AD105">
         <v>66</v>
@@ -13370,25 +13370,25 @@
         <v>14</v>
       </c>
       <c r="AG105">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AH105">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AI105">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AJ105">
-        <v>1.398</v>
+        <v>1.39</v>
       </c>
       <c r="AK105">
-        <v>0.355</v>
+        <v>0.354</v>
       </c>
       <c r="AL105">
-        <v>11</v>
+        <v>10.9</v>
       </c>
       <c r="AM105">
-        <v>2.84</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="106" spans="1:39">
@@ -14211,34 +14211,34 @@
         <v>27</v>
       </c>
       <c r="E113">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F113">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G113">
         <v>4</v>
       </c>
       <c r="H113">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J113">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="K113">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="L113">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="M113">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N113">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O113">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="P113">
         <v>8</v>
@@ -14247,13 +14247,13 @@
         <v>3</v>
       </c>
       <c r="R113">
-        <v>4.5</v>
+        <v>4.65</v>
       </c>
       <c r="S113">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="T113">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="U113">
         <v>1</v>
@@ -14265,22 +14265,22 @@
         <v>5</v>
       </c>
       <c r="X113">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y113">
         <v>1</v>
       </c>
       <c r="Z113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA113">
         <v>0</v>
       </c>
       <c r="AB113">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="AC113">
-        <v>894</v>
+        <v>977</v>
       </c>
       <c r="AD113">
         <v>68</v>
@@ -14292,25 +14292,25 @@
         <v>11</v>
       </c>
       <c r="AG113">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AH113">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AI113">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AJ113">
-        <v>1.148</v>
+        <v>1.133</v>
       </c>
       <c r="AK113">
-        <v>0.294</v>
+        <v>0.288</v>
       </c>
       <c r="AL113">
-        <v>9.300000000000001</v>
+        <v>8.9</v>
       </c>
       <c r="AM113">
-        <v>4.67</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="114" spans="1:39">
@@ -15258,49 +15258,49 @@
         <v>26</v>
       </c>
       <c r="E122">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F122">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G122">
         <v>8</v>
       </c>
       <c r="H122">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J122">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="K122">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="L122">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M122">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="N122">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O122">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="P122">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="Q122">
         <v>6</v>
       </c>
       <c r="R122">
-        <v>4.17</v>
+        <v>4.66</v>
       </c>
       <c r="S122">
-        <v>410</v>
+        <v>430</v>
       </c>
       <c r="T122">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="U122">
         <v>0</v>
@@ -15324,10 +15324,10 @@
         <v>0</v>
       </c>
       <c r="AB122">
-        <v>458</v>
+        <v>480</v>
       </c>
       <c r="AC122">
-        <v>1747</v>
+        <v>1834</v>
       </c>
       <c r="AD122">
         <v>65</v>
@@ -15339,25 +15339,25 @@
         <v>11</v>
       </c>
       <c r="AG122">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AH122">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AI122">
         <v>9</v>
       </c>
       <c r="AJ122">
-        <v>1.255</v>
+        <v>1.298</v>
       </c>
       <c r="AK122">
-        <v>0.282</v>
+        <v>0.289</v>
       </c>
       <c r="AL122">
         <v>8.800000000000001</v>
       </c>
       <c r="AM122">
-        <v>2.68</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="123" spans="1:39">
@@ -16299,7 +16299,7 @@
         <v>27</v>
       </c>
       <c r="E131">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F131">
         <v>0</v>
@@ -16311,19 +16311,19 @@
         <v>4</v>
       </c>
       <c r="J131">
-        <v>41.2</v>
+        <v>42</v>
       </c>
       <c r="K131">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L131">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M131">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N131">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O131">
         <v>42</v>
@@ -16335,13 +16335,13 @@
         <v>0</v>
       </c>
       <c r="R131">
-        <v>3.46</v>
+        <v>3.64</v>
       </c>
       <c r="S131">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="T131">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U131">
         <v>0</v>
@@ -16365,10 +16365,10 @@
         <v>0</v>
       </c>
       <c r="AB131">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="AC131">
-        <v>654</v>
+        <v>663</v>
       </c>
       <c r="AD131">
         <v>66</v>
@@ -16380,25 +16380,25 @@
         <v>13</v>
       </c>
       <c r="AG131">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AH131">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AI131">
         <v>4</v>
       </c>
       <c r="AJ131">
-        <v>1.368</v>
+        <v>1.429</v>
       </c>
       <c r="AK131">
-        <v>0.333</v>
+        <v>0.342</v>
       </c>
       <c r="AL131">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="AM131">
-        <v>2.47</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="132" spans="1:39">
@@ -16647,49 +16647,49 @@
         <v>29</v>
       </c>
       <c r="E134">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F134">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G134">
         <v>7</v>
       </c>
       <c r="H134">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J134">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="K134">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="L134">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M134">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="N134">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O134">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="P134">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q134">
         <v>3</v>
       </c>
       <c r="R134">
-        <v>5.4</v>
+        <v>5.58</v>
       </c>
       <c r="S134">
-        <v>445</v>
+        <v>470</v>
       </c>
       <c r="T134">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="U134">
         <v>3</v>
@@ -16713,10 +16713,10 @@
         <v>1</v>
       </c>
       <c r="AB134">
-        <v>496</v>
+        <v>522</v>
       </c>
       <c r="AC134">
-        <v>1894</v>
+        <v>1981</v>
       </c>
       <c r="AD134">
         <v>63</v>
@@ -16731,13 +16731,13 @@
         <v>42</v>
       </c>
       <c r="AH134">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AI134">
         <v>2</v>
       </c>
       <c r="AJ134">
-        <v>1.374</v>
+        <v>1.372</v>
       </c>
       <c r="AK134">
         <v>0.291</v>
@@ -16746,7 +16746,7 @@
         <v>8.6</v>
       </c>
       <c r="AM134">
-        <v>2.44</v>
+        <v>2.52</v>
       </c>
     </row>
     <row r="135" spans="1:39">
@@ -17691,7 +17691,7 @@
         <v>29</v>
       </c>
       <c r="E143">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F143">
         <v>0</v>
@@ -17700,7 +17700,7 @@
         <v>1</v>
       </c>
       <c r="J143">
-        <v>17.2</v>
+        <v>19</v>
       </c>
       <c r="K143">
         <v>17</v>
@@ -17715,7 +17715,7 @@
         <v>7</v>
       </c>
       <c r="O143">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P143">
         <v>2</v>
@@ -17724,52 +17724,52 @@
         <v>0</v>
       </c>
       <c r="R143">
-        <v>6.11</v>
+        <v>5.68</v>
       </c>
       <c r="S143">
+        <v>70</v>
+      </c>
+      <c r="T143">
+        <v>1</v>
+      </c>
+      <c r="U143">
+        <v>1</v>
+      </c>
+      <c r="V143">
+        <v>0</v>
+      </c>
+      <c r="W143">
+        <v>1</v>
+      </c>
+      <c r="X143">
+        <v>2</v>
+      </c>
+      <c r="Y143">
+        <v>1</v>
+      </c>
+      <c r="Z143">
+        <v>0</v>
+      </c>
+      <c r="AA143">
+        <v>0</v>
+      </c>
+      <c r="AB143">
+        <v>79</v>
+      </c>
+      <c r="AC143">
+        <v>288</v>
+      </c>
+      <c r="AD143">
         <v>66</v>
-      </c>
-      <c r="T143">
-        <v>1</v>
-      </c>
-      <c r="U143">
-        <v>1</v>
-      </c>
-      <c r="V143">
-        <v>0</v>
-      </c>
-      <c r="W143">
-        <v>1</v>
-      </c>
-      <c r="X143">
-        <v>2</v>
-      </c>
-      <c r="Y143">
-        <v>1</v>
-      </c>
-      <c r="Z143">
-        <v>0</v>
-      </c>
-      <c r="AA143">
-        <v>0</v>
-      </c>
-      <c r="AB143">
-        <v>75</v>
-      </c>
-      <c r="AC143">
-        <v>269</v>
-      </c>
-      <c r="AD143">
-        <v>65</v>
       </c>
       <c r="AE143">
         <v>17</v>
       </c>
       <c r="AF143">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AG143">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AH143">
         <v>25</v>
@@ -17778,16 +17778,16 @@
         <v>10</v>
       </c>
       <c r="AJ143">
-        <v>1.358</v>
+        <v>1.263</v>
       </c>
       <c r="AK143">
-        <v>0.263</v>
+        <v>0.254</v>
       </c>
       <c r="AL143">
-        <v>4.6</v>
+        <v>5.2</v>
       </c>
       <c r="AM143">
-        <v>1.29</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="144" spans="1:39">
@@ -17804,52 +17804,52 @@
         <v>28</v>
       </c>
       <c r="E144">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F144">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G144">
         <v>7</v>
       </c>
       <c r="H144">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J144">
+        <v>102.1</v>
+      </c>
+      <c r="K144">
         <v>100</v>
       </c>
-      <c r="K144">
-        <v>95</v>
-      </c>
       <c r="L144">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="M144">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="N144">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O144">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P144">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q144">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R144">
-        <v>4.32</v>
+        <v>4.84</v>
       </c>
       <c r="S144">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="T144">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="U144">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V144">
         <v>0</v>
@@ -17870,10 +17870,10 @@
         <v>0</v>
       </c>
       <c r="AB144">
-        <v>429</v>
+        <v>444</v>
       </c>
       <c r="AC144">
-        <v>1710</v>
+        <v>1767</v>
       </c>
       <c r="AD144">
         <v>62</v>
@@ -17894,16 +17894,16 @@
         <v>7</v>
       </c>
       <c r="AJ144">
-        <v>1.35</v>
+        <v>1.388</v>
       </c>
       <c r="AK144">
-        <v>0.3</v>
+        <v>0.303</v>
       </c>
       <c r="AL144">
-        <v>8.300000000000001</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="AM144">
-        <v>2.3</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="145" spans="1:39">
@@ -17920,10 +17920,10 @@
         <v>28</v>
       </c>
       <c r="E145">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F145">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G145">
         <v>7</v>
@@ -17932,22 +17932,22 @@
         <v>5</v>
       </c>
       <c r="J145">
-        <v>116</v>
+        <v>119.2</v>
       </c>
       <c r="K145">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="L145">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="M145">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="N145">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="O145">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="P145">
         <v>22</v>
@@ -17956,13 +17956,13 @@
         <v>4</v>
       </c>
       <c r="R145">
-        <v>4.58</v>
+        <v>4.81</v>
       </c>
       <c r="S145">
-        <v>452</v>
+        <v>468</v>
       </c>
       <c r="T145">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U145">
         <v>2</v>
@@ -17971,7 +17971,7 @@
         <v>0</v>
       </c>
       <c r="W145">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X145">
         <v>0</v>
@@ -17986,10 +17986,10 @@
         <v>0</v>
       </c>
       <c r="AB145">
-        <v>494</v>
+        <v>513</v>
       </c>
       <c r="AC145">
-        <v>1861</v>
+        <v>1933</v>
       </c>
       <c r="AD145">
         <v>65</v>
@@ -18010,16 +18010,16 @@
         <v>5</v>
       </c>
       <c r="AJ145">
-        <v>1.293</v>
+        <v>1.329</v>
       </c>
       <c r="AK145">
-        <v>0.259</v>
+        <v>0.265</v>
       </c>
       <c r="AL145">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="AM145">
-        <v>2.18</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="146" spans="1:39">
@@ -18610,7 +18610,7 @@
         <v>27</v>
       </c>
       <c r="E151">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F151">
         <v>1</v>
@@ -18622,7 +18622,7 @@
         <v>1</v>
       </c>
       <c r="J151">
-        <v>38.1</v>
+        <v>39.1</v>
       </c>
       <c r="K151">
         <v>46</v>
@@ -18637,7 +18637,7 @@
         <v>10</v>
       </c>
       <c r="O151">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="P151">
         <v>4</v>
@@ -18646,10 +18646,10 @@
         <v>0</v>
       </c>
       <c r="R151">
-        <v>3.05</v>
+        <v>2.97</v>
       </c>
       <c r="S151">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="T151">
         <v>9</v>
@@ -18676,10 +18676,10 @@
         <v>0</v>
       </c>
       <c r="AB151">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AC151">
-        <v>578</v>
+        <v>592</v>
       </c>
       <c r="AD151">
         <v>68</v>
@@ -18691,25 +18691,25 @@
         <v>7</v>
       </c>
       <c r="AG151">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH151">
         <v>24</v>
       </c>
       <c r="AI151">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AJ151">
-        <v>1.461</v>
+        <v>1.424</v>
       </c>
       <c r="AK151">
-        <v>0.321</v>
+        <v>0.318</v>
       </c>
       <c r="AL151">
-        <v>4.2</v>
+        <v>4.6</v>
       </c>
       <c r="AM151">
-        <v>1.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:39">
@@ -19297,40 +19297,40 @@
         <v>30</v>
       </c>
       <c r="E157">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F157">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J157">
+        <v>12</v>
+      </c>
+      <c r="K157">
         <v>9</v>
       </c>
-      <c r="K157">
-        <v>5</v>
-      </c>
       <c r="L157">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M157">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N157">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O157">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="P157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q157">
         <v>0</v>
       </c>
       <c r="R157">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="S157">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="T157">
         <v>0</v>
@@ -19357,10 +19357,10 @@
         <v>0</v>
       </c>
       <c r="AB157">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AC157">
-        <v>140</v>
+        <v>186</v>
       </c>
       <c r="AD157">
         <v>67</v>
@@ -19372,25 +19372,25 @@
         <v>14</v>
       </c>
       <c r="AG157">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AH157">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="AI157">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="AJ157">
-        <v>0.778</v>
+        <v>1</v>
       </c>
       <c r="AK157">
-        <v>0.238</v>
+        <v>0.267</v>
       </c>
       <c r="AL157">
-        <v>10</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="AM157">
-        <v>5</v>
+        <v>4.33</v>
       </c>
     </row>
     <row r="158" spans="1:39">
@@ -20790,34 +20790,34 @@
         <v>29</v>
       </c>
       <c r="E170">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F170">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G170">
         <v>5</v>
       </c>
       <c r="H170">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J170">
-        <v>100.2</v>
+        <v>103.2</v>
       </c>
       <c r="K170">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L170">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M170">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N170">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="O170">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="P170">
         <v>19</v>
@@ -20826,10 +20826,10 @@
         <v>3</v>
       </c>
       <c r="R170">
-        <v>4.65</v>
+        <v>4.77</v>
       </c>
       <c r="S170">
-        <v>376</v>
+        <v>391</v>
       </c>
       <c r="T170">
         <v>15</v>
@@ -20856,10 +20856,10 @@
         <v>0</v>
       </c>
       <c r="AB170">
-        <v>420</v>
+        <v>438</v>
       </c>
       <c r="AC170">
-        <v>1746</v>
+        <v>1824</v>
       </c>
       <c r="AD170">
         <v>64</v>
@@ -20880,16 +20880,16 @@
         <v>8</v>
       </c>
       <c r="AJ170">
-        <v>1.242</v>
+        <v>1.293</v>
       </c>
       <c r="AK170">
-        <v>0.282</v>
+        <v>0.296</v>
       </c>
       <c r="AL170">
-        <v>11.1</v>
+        <v>11.3</v>
       </c>
       <c r="AM170">
-        <v>3.1</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="171" spans="1:39">
@@ -23086,7 +23086,7 @@
         <v>30</v>
       </c>
       <c r="E190">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F190">
         <v>1</v>
@@ -23101,37 +23101,37 @@
         <v>1</v>
       </c>
       <c r="J190">
-        <v>36.2</v>
+        <v>39.2</v>
       </c>
       <c r="K190">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="L190">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M190">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="N190">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O190">
         <v>19</v>
       </c>
       <c r="P190">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q190">
         <v>0</v>
       </c>
       <c r="R190">
-        <v>1.47</v>
+        <v>2.5</v>
       </c>
       <c r="S190">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="T190">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U190">
         <v>0</v>
@@ -23155,40 +23155,40 @@
         <v>0</v>
       </c>
       <c r="AB190">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="AC190">
-        <v>542</v>
+        <v>601</v>
       </c>
       <c r="AD190">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AE190">
         <v>15</v>
       </c>
       <c r="AF190">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AG190">
         <v>38</v>
       </c>
       <c r="AH190">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AI190">
         <v>6</v>
       </c>
       <c r="AJ190">
-        <v>0.927</v>
+        <v>1.059</v>
       </c>
       <c r="AK190">
-        <v>0.187</v>
+        <v>0.207</v>
       </c>
       <c r="AL190">
-        <v>4.7</v>
+        <v>4.3</v>
       </c>
       <c r="AM190">
-        <v>1.73</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="191" spans="1:39">
@@ -23431,7 +23431,7 @@
         <v>33</v>
       </c>
       <c r="E193">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F193">
         <v>0</v>
@@ -23446,7 +23446,7 @@
         <v>6</v>
       </c>
       <c r="J193">
-        <v>39.1</v>
+        <v>40.1</v>
       </c>
       <c r="K193">
         <v>33</v>
@@ -23458,10 +23458,10 @@
         <v>14</v>
       </c>
       <c r="N193">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O193">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P193">
         <v>4</v>
@@ -23470,10 +23470,10 @@
         <v>0</v>
       </c>
       <c r="R193">
-        <v>3.2</v>
+        <v>3.12</v>
       </c>
       <c r="S193">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="T193">
         <v>7</v>
@@ -23500,10 +23500,10 @@
         <v>0</v>
       </c>
       <c r="AB193">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="AC193">
-        <v>641</v>
+        <v>658</v>
       </c>
       <c r="AD193">
         <v>69</v>
@@ -23515,25 +23515,25 @@
         <v>12</v>
       </c>
       <c r="AG193">
+        <v>24</v>
+      </c>
+      <c r="AH193">
         <v>25</v>
-      </c>
-      <c r="AH193">
-        <v>26</v>
       </c>
       <c r="AI193">
         <v>17</v>
       </c>
       <c r="AJ193">
-        <v>1.144</v>
+        <v>1.14</v>
       </c>
       <c r="AK193">
-        <v>0.293</v>
+        <v>0.287</v>
       </c>
       <c r="AL193">
         <v>10.3</v>
       </c>
       <c r="AM193">
-        <v>3.75</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="194" spans="1:39">
@@ -23666,10 +23666,10 @@
         <v>30</v>
       </c>
       <c r="E195">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F195">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G195">
         <v>6</v>
@@ -23678,22 +23678,22 @@
         <v>6</v>
       </c>
       <c r="J195">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="K195">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="L195">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="M195">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N195">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O195">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="P195">
         <v>17</v>
@@ -23702,13 +23702,13 @@
         <v>8</v>
       </c>
       <c r="R195">
-        <v>6.12</v>
+        <v>5.72</v>
       </c>
       <c r="S195">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="T195">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="U195">
         <v>1</v>
@@ -23717,13 +23717,13 @@
         <v>0</v>
       </c>
       <c r="W195">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="X195">
         <v>2</v>
       </c>
       <c r="Y195">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Z195">
         <v>1</v>
@@ -23732,13 +23732,13 @@
         <v>3</v>
       </c>
       <c r="AB195">
-        <v>355</v>
+        <v>381</v>
       </c>
       <c r="AC195">
-        <v>1389</v>
+        <v>1478</v>
       </c>
       <c r="AD195">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AE195">
         <v>17</v>
@@ -23747,7 +23747,7 @@
         <v>8</v>
       </c>
       <c r="AG195">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AH195">
         <v>25</v>
@@ -23756,16 +23756,16 @@
         <v>6</v>
       </c>
       <c r="AJ195">
-        <v>1.564</v>
+        <v>1.518</v>
       </c>
       <c r="AK195">
-        <v>0.303</v>
+        <v>0.302</v>
       </c>
       <c r="AL195">
-        <v>7.3</v>
+        <v>7.1</v>
       </c>
       <c r="AM195">
-        <v>1.8</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="196" spans="1:39">
@@ -24130,10 +24130,10 @@
         <v>35</v>
       </c>
       <c r="E199">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F199">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G199">
         <v>7</v>
@@ -24142,37 +24142,37 @@
         <v>5</v>
       </c>
       <c r="J199">
-        <v>99.09999999999999</v>
+        <v>103</v>
       </c>
       <c r="K199">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="L199">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="M199">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="N199">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="O199">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="P199">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q199">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R199">
-        <v>4.44</v>
+        <v>4.54</v>
       </c>
       <c r="S199">
-        <v>394</v>
+        <v>412</v>
       </c>
       <c r="T199">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="U199">
         <v>1</v>
@@ -24196,10 +24196,10 @@
         <v>0</v>
       </c>
       <c r="AB199">
-        <v>422</v>
+        <v>445</v>
       </c>
       <c r="AC199">
-        <v>1575</v>
+        <v>1665</v>
       </c>
       <c r="AD199">
         <v>63</v>
@@ -24220,16 +24220,16 @@
         <v>7</v>
       </c>
       <c r="AJ199">
-        <v>1.299</v>
+        <v>1.35</v>
       </c>
       <c r="AK199">
-        <v>0.277</v>
+        <v>0.281</v>
       </c>
       <c r="AL199">
-        <v>5.3</v>
+        <v>5.5</v>
       </c>
       <c r="AM199">
-        <v>2.68</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="200" spans="1:39">
@@ -25058,34 +25058,34 @@
         <v>32</v>
       </c>
       <c r="E207">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F207">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G207">
         <v>10</v>
       </c>
       <c r="H207">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J207">
-        <v>119.2</v>
+        <v>124.2</v>
       </c>
       <c r="K207">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="L207">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M207">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N207">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="O207">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="P207">
         <v>15</v>
@@ -25094,13 +25094,13 @@
         <v>4</v>
       </c>
       <c r="R207">
-        <v>3.08</v>
+        <v>3.1</v>
       </c>
       <c r="S207">
-        <v>430</v>
+        <v>452</v>
       </c>
       <c r="T207">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="U207">
         <v>0</v>
@@ -25124,10 +25124,10 @@
         <v>1</v>
       </c>
       <c r="AB207">
-        <v>478</v>
+        <v>505</v>
       </c>
       <c r="AC207">
-        <v>1934</v>
+        <v>2041</v>
       </c>
       <c r="AD207">
         <v>62</v>
@@ -25148,16 +25148,16 @@
         <v>7</v>
       </c>
       <c r="AJ207">
-        <v>1.003</v>
+        <v>1.051</v>
       </c>
       <c r="AK207">
-        <v>0.228</v>
+        <v>0.234</v>
       </c>
       <c r="AL207">
-        <v>10.2</v>
+        <v>10</v>
       </c>
       <c r="AM207">
-        <v>3.29</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="208" spans="1:39">
@@ -26331,46 +26331,46 @@
         <v>31</v>
       </c>
       <c r="E218">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F218">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H218">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J218">
-        <v>28.2</v>
+        <v>34.1</v>
       </c>
       <c r="K218">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="L218">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M218">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N218">
         <v>7</v>
       </c>
       <c r="O218">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="P218">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q218">
         <v>0</v>
       </c>
       <c r="R218">
-        <v>5.65</v>
+        <v>6.03</v>
       </c>
       <c r="S218">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="T218">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="U218">
         <v>2</v>
@@ -26382,10 +26382,10 @@
         <v>2</v>
       </c>
       <c r="X218">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y218">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z218">
         <v>1</v>
@@ -26394,10 +26394,10 @@
         <v>0</v>
       </c>
       <c r="AB218">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="AC218">
-        <v>493</v>
+        <v>580</v>
       </c>
       <c r="AD218">
         <v>67</v>
@@ -26406,28 +26406,28 @@
         <v>16</v>
       </c>
       <c r="AF218">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AG218">
         <v>34</v>
       </c>
       <c r="AH218">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AI218">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AJ218">
-        <v>1.605</v>
+        <v>1.66</v>
       </c>
       <c r="AK218">
-        <v>0.324</v>
+        <v>0.35</v>
       </c>
       <c r="AL218">
-        <v>4.4</v>
+        <v>5.2</v>
       </c>
       <c r="AM218">
-        <v>2</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="219" spans="1:39">
@@ -27259,55 +27259,55 @@
         <v>34</v>
       </c>
       <c r="E226">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F226">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G226">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H226">
         <v>7</v>
       </c>
       <c r="J226">
-        <v>109.2</v>
+        <v>116.2</v>
       </c>
       <c r="K226">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="L226">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M226">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N226">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O226">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="P226">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q226">
         <v>3</v>
       </c>
       <c r="R226">
-        <v>4.19</v>
+        <v>4.01</v>
       </c>
       <c r="S226">
-        <v>408</v>
+        <v>433</v>
       </c>
       <c r="T226">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U226">
         <v>1</v>
       </c>
       <c r="V226">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W226">
         <v>5</v>
@@ -27316,7 +27316,7 @@
         <v>3</v>
       </c>
       <c r="Y226">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Z226">
         <v>1</v>
@@ -27325,16 +27325,16 @@
         <v>0</v>
       </c>
       <c r="AB226">
-        <v>451</v>
+        <v>478</v>
       </c>
       <c r="AC226">
-        <v>1806</v>
+        <v>1892</v>
       </c>
       <c r="AD226">
         <v>67</v>
       </c>
       <c r="AE226">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AF226">
         <v>12</v>
@@ -27343,22 +27343,22 @@
         <v>34</v>
       </c>
       <c r="AH226">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AI226">
         <v>7</v>
       </c>
       <c r="AJ226">
-        <v>1.158</v>
+        <v>1.14</v>
       </c>
       <c r="AK226">
-        <v>0.27</v>
+        <v>0.265</v>
       </c>
       <c r="AL226">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="AM226">
-        <v>3.06</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="227" spans="1:39">
@@ -28190,10 +28190,10 @@
         <v>35</v>
       </c>
       <c r="E234">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F234">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G234">
         <v>9</v>
@@ -28202,37 +28202,37 @@
         <v>3</v>
       </c>
       <c r="J234">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="K234">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="L234">
+        <v>36</v>
+      </c>
+      <c r="M234">
         <v>34</v>
-      </c>
-      <c r="M234">
-        <v>32</v>
       </c>
       <c r="N234">
         <v>26</v>
       </c>
       <c r="O234">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P234">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q234">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R234">
-        <v>2.36</v>
+        <v>2.39</v>
       </c>
       <c r="S234">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="T234">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="U234">
         <v>1</v>
@@ -28241,31 +28241,31 @@
         <v>0</v>
       </c>
       <c r="W234">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X234">
         <v>1</v>
       </c>
       <c r="Y234">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z234">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA234">
         <v>1</v>
       </c>
       <c r="AB234">
-        <v>467</v>
+        <v>491</v>
       </c>
       <c r="AC234">
-        <v>1908</v>
+        <v>2013</v>
       </c>
       <c r="AD234">
         <v>65</v>
       </c>
       <c r="AE234">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AF234">
         <v>14</v>
@@ -28280,16 +28280,16 @@
         <v>7</v>
       </c>
       <c r="AJ234">
-        <v>0.861</v>
+        <v>0.875</v>
       </c>
       <c r="AK234">
-        <v>0.244</v>
+        <v>0.255</v>
       </c>
       <c r="AL234">
-        <v>11.4</v>
+        <v>11.5</v>
       </c>
       <c r="AM234">
-        <v>5.92</v>
+        <v>6.31</v>
       </c>
     </row>
     <row r="235" spans="1:39">
@@ -28877,10 +28877,10 @@
         <v>35</v>
       </c>
       <c r="E240">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F240">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G240">
         <v>2</v>
@@ -28889,34 +28889,34 @@
         <v>6</v>
       </c>
       <c r="J240">
-        <v>101.2</v>
+        <v>107.2</v>
       </c>
       <c r="K240">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="L240">
+        <v>57</v>
+      </c>
+      <c r="M240">
         <v>53</v>
       </c>
-      <c r="M240">
-        <v>49</v>
-      </c>
       <c r="N240">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="O240">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="P240">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q240">
         <v>3</v>
       </c>
       <c r="R240">
-        <v>4.34</v>
+        <v>4.43</v>
       </c>
       <c r="S240">
-        <v>402</v>
+        <v>424</v>
       </c>
       <c r="T240">
         <v>25</v>
@@ -28943,10 +28943,10 @@
         <v>1</v>
       </c>
       <c r="AB240">
-        <v>448</v>
+        <v>475</v>
       </c>
       <c r="AC240">
-        <v>1754</v>
+        <v>1841</v>
       </c>
       <c r="AD240">
         <v>64</v>
@@ -28955,28 +28955,28 @@
         <v>15</v>
       </c>
       <c r="AF240">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AG240">
         <v>31</v>
       </c>
       <c r="AH240">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AI240">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AJ240">
-        <v>1.407</v>
+        <v>1.412</v>
       </c>
       <c r="AK240">
-        <v>0.283</v>
+        <v>0.278</v>
       </c>
       <c r="AL240">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="AM240">
-        <v>2.1</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="241" spans="1:39">

</xml_diff>